<commit_message>
gửi AC ngay ko cần quá 30p
</commit_message>
<xml_diff>
--- a/fms_data.xlsx
+++ b/fms_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="57">
   <si>
     <t>STT</t>
   </si>
@@ -103,58 +103,88 @@
     <t>TG Tạo Trên FM</t>
   </si>
   <si>
-    <t>SR_TTT032M_HNI</t>
-  </si>
-  <si>
-    <t>3G_QOI083S_HNI</t>
-  </si>
-  <si>
-    <t>SR_BVI001M_HNI</t>
-  </si>
-  <si>
-    <t>Thon-Dan-Lap-TTT_HNI</t>
-  </si>
-  <si>
-    <t>PHUONG-CACH-THON4-SMC-QOI_HNI</t>
-  </si>
-  <si>
-    <t>BD-Tay-Dang-BVI_HNI</t>
+    <t>SR_BVI027M_HNI</t>
+  </si>
+  <si>
+    <t>UL_BVI133M_HNI</t>
+  </si>
+  <si>
+    <t>UL_DPG058M_HNI</t>
+  </si>
+  <si>
+    <t>2G_BVI010M_HNI</t>
+  </si>
+  <si>
+    <t>3G_BVI010M_HNI</t>
+  </si>
+  <si>
+    <t>4G-BVI010M-HNI</t>
+  </si>
+  <si>
+    <t>SR_BVI010M_HNI</t>
+  </si>
+  <si>
+    <t>Thon-Lien-Tong-BVI_HNI</t>
+  </si>
+  <si>
+    <t>TONG-BAT-THON-TONG-LENH-BVI_HNI</t>
+  </si>
+  <si>
+    <t>KCN-CAU-GAO-DPG_HNI</t>
+  </si>
+  <si>
+    <t>Cam-Thuong-Thon-Van-Minh-BVI_HNI</t>
   </si>
   <si>
     <t>POWER_AC_EAS</t>
   </si>
   <si>
-    <t>SITE_OOS</t>
-  </si>
-  <si>
-    <t>17/04/2025 14:54:48</t>
-  </si>
-  <si>
-    <t>17/04/2025 06:59:22</t>
-  </si>
-  <si>
-    <t>16/04/2025 10:00:24</t>
-  </si>
-  <si>
-    <t>Thạch Thất</t>
-  </si>
-  <si>
-    <t>Quốc Oai</t>
+    <t>SITE_OOS_BY_POWER</t>
+  </si>
+  <si>
+    <t>06/05/2025 15:42:22</t>
+  </si>
+  <si>
+    <t>06/05/2025 15:37:25</t>
+  </si>
+  <si>
+    <t>06/05/2025 14:30:14</t>
+  </si>
+  <si>
+    <t>06/05/2025 13:42:12</t>
+  </si>
+  <si>
+    <t>06/05/2025 13:41:56</t>
+  </si>
+  <si>
+    <t>06/05/2025 13:41:51</t>
+  </si>
+  <si>
+    <t>06/05/2025 06:18:28</t>
   </si>
   <si>
     <t>Ba Vì</t>
   </si>
   <si>
-    <t>Trạm smc mất điện - 1 - sonnn - 17/04/2025 07:02:36</t>
+    <t>Đan Phượng</t>
+  </si>
+  <si>
+    <t>184205 - VTHN TĐML - HNI dựng lại côt thay cáp - 4 - thainh1 - 06/05/2025 13:56:39</t>
+  </si>
+  <si>
+    <t>184205 - VTHN TĐML - HNI dựng lại côt thay cáp - 4 - thainh1 - 06/05/2025 13:56:40</t>
+  </si>
+  <si>
+    <t>Mất nguồn AC - 1 - huongvl1 - 06/05/2025 10:23:32</t>
+  </si>
+  <si>
+    <t>Trạm viễn thông loại 1</t>
+  </si>
+  <si>
+    <t>Trạm viễn thông loại 3</t>
   </si>
   <si>
     <t>Trạm viễn thông loại 2</t>
-  </si>
-  <si>
-    <t>Trạm viễn thông loại 3</t>
-  </si>
-  <si>
-    <t>Trạm viễn thông loại 1</t>
   </si>
 </sst>
 </file>
@@ -521,7 +551,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -533,10 +563,10 @@
     <col min="4" max="4" width="5.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" customWidth="1"/>
@@ -547,7 +577,7 @@
     <col min="19" max="19" width="9.7109375" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="13.7109375" customWidth="1"/>
-    <col min="22" max="22" width="53.7109375" customWidth="1"/>
+    <col min="22" max="22" width="84.7109375" customWidth="1"/>
     <col min="23" max="23" width="12.7109375" customWidth="1"/>
     <col min="24" max="24" width="9.7109375" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" customWidth="1"/>
@@ -656,16 +686,16 @@
         <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -675,7 +705,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -684,7 +714,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
@@ -699,16 +729,16 @@
         <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -718,18 +748,16 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="U3" s="2"/>
-      <c r="V3" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
@@ -744,16 +772,16 @@
         <v>31</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -763,7 +791,7 @@
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
@@ -772,10 +800,190 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+    </row>
+    <row r="6" spans="1:29">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+    </row>
+    <row r="7" spans="1:29">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+    </row>
+    <row r="8" spans="1:29">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W8" s="2"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="2"/>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sua ban ton zalo
</commit_message>
<xml_diff>
--- a/fms_data.xlsx
+++ b/fms_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>STT</t>
   </si>
@@ -103,88 +103,40 @@
     <t>TG Tạo Trên FM</t>
   </si>
   <si>
-    <t>SR_BVI027M_HNI</t>
-  </si>
-  <si>
-    <t>UL_BVI133M_HNI</t>
-  </si>
-  <si>
-    <t>UL_DPG058M_HNI</t>
-  </si>
-  <si>
-    <t>2G_BVI010M_HNI</t>
-  </si>
-  <si>
-    <t>3G_BVI010M_HNI</t>
-  </si>
-  <si>
-    <t>4G-BVI010M-HNI</t>
-  </si>
-  <si>
-    <t>SR_BVI010M_HNI</t>
-  </si>
-  <si>
-    <t>Thon-Lien-Tong-BVI_HNI</t>
-  </si>
-  <si>
-    <t>TONG-BAT-THON-TONG-LENH-BVI_HNI</t>
-  </si>
-  <si>
-    <t>KCN-CAU-GAO-DPG_HNI</t>
-  </si>
-  <si>
-    <t>Cam-Thuong-Thon-Van-Minh-BVI_HNI</t>
+    <t>UL_TTT093M_HNI</t>
+  </si>
+  <si>
+    <t>3G_DPG045S_HNI</t>
+  </si>
+  <si>
+    <t>THACH-HOA-TTT_HNI</t>
+  </si>
+  <si>
+    <t>TRUNG-CHAU-VAN-MON2-11-SMC-DPG_HNI</t>
   </si>
   <si>
     <t>POWER_AC_EAS</t>
   </si>
   <si>
-    <t>SITE_OOS_BY_POWER</t>
-  </si>
-  <si>
-    <t>06/05/2025 15:42:22</t>
-  </si>
-  <si>
-    <t>06/05/2025 15:37:25</t>
-  </si>
-  <si>
-    <t>06/05/2025 14:30:14</t>
-  </si>
-  <si>
-    <t>06/05/2025 13:42:12</t>
-  </si>
-  <si>
-    <t>06/05/2025 13:41:56</t>
-  </si>
-  <si>
-    <t>06/05/2025 13:41:51</t>
-  </si>
-  <si>
-    <t>06/05/2025 06:18:28</t>
-  </si>
-  <si>
-    <t>Ba Vì</t>
+    <t>SITE_OOS</t>
+  </si>
+  <si>
+    <t>07/05/2025 13:18:36</t>
+  </si>
+  <si>
+    <t>06/05/2025 23:18:18</t>
+  </si>
+  <si>
+    <t>Thạch Thất</t>
   </si>
   <si>
     <t>Đan Phượng</t>
   </si>
   <si>
-    <t>184205 - VTHN TĐML - HNI dựng lại côt thay cáp - 4 - thainh1 - 06/05/2025 13:56:39</t>
-  </si>
-  <si>
-    <t>184205 - VTHN TĐML - HNI dựng lại côt thay cáp - 4 - thainh1 - 06/05/2025 13:56:40</t>
-  </si>
-  <si>
-    <t>Mất nguồn AC - 1 - huongvl1 - 06/05/2025 10:23:32</t>
-  </si>
-  <si>
-    <t>Trạm viễn thông loại 1</t>
+    <t>Trạm smc mất điện - 1 - sonnn - 06/05/2025 23:24:34</t>
   </si>
   <si>
     <t>Trạm viễn thông loại 3</t>
-  </si>
-  <si>
-    <t>Trạm viễn thông loại 2</t>
   </si>
 </sst>
 </file>
@@ -551,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC8"/>
+  <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -563,10 +515,10 @@
     <col min="4" max="4" width="5.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="34.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" customWidth="1"/>
     <col min="12" max="12" width="21.7109375" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" customWidth="1"/>
@@ -577,7 +529,7 @@
     <col min="19" max="19" width="9.7109375" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="13.7109375" customWidth="1"/>
-    <col min="22" max="22" width="84.7109375" customWidth="1"/>
+    <col min="22" max="22" width="53.7109375" customWidth="1"/>
     <col min="23" max="23" width="12.7109375" customWidth="1"/>
     <col min="24" max="24" width="9.7109375" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" customWidth="1"/>
@@ -686,16 +638,16 @@
         <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -705,7 +657,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -714,7 +666,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
@@ -729,16 +681,16 @@
         <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -748,242 +700,21 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="V3" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
-    </row>
-    <row r="4" spans="1:29">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-    </row>
-    <row r="5" spans="1:29">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-    </row>
-    <row r="6" spans="1:29">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-    </row>
-    <row r="7" spans="1:29">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
-      <c r="AA7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB7" s="2"/>
-      <c r="AC7" s="2"/>
-    </row>
-    <row r="8" spans="1:29">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
-      <c r="AA8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB8" s="2"/>
-      <c r="AC8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
loai tru trạm sty003
</commit_message>
<xml_diff>
--- a/fms_data.xlsx
+++ b/fms_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
   <si>
     <t>STT</t>
   </si>
@@ -103,16 +103,25 @@
     <t>TG Tạo Trên FM</t>
   </si>
   <si>
+    <t>SR_PTO016M_HNI</t>
+  </si>
+  <si>
     <t>UL_TTT093M_HNI</t>
   </si>
   <si>
-    <t>3G_DPG045S_HNI</t>
+    <t>4G-STY003M-HNI</t>
+  </si>
+  <si>
+    <t>3G_STY003M_HNI</t>
+  </si>
+  <si>
+    <t>Tam-Hiep-Thon-Thuong-PTO_HNI</t>
   </si>
   <si>
     <t>THACH-HOA-TTT_HNI</t>
   </si>
   <si>
-    <t>TRUNG-CHAU-VAN-MON2-11-SMC-DPG_HNI</t>
+    <t>Lang-Van-Hoa-STY_HNI</t>
   </si>
   <si>
     <t>POWER_AC_EAS</t>
@@ -121,22 +130,40 @@
     <t>SITE_OOS</t>
   </si>
   <si>
-    <t>07/05/2025 14:13:49</t>
-  </si>
-  <si>
-    <t>06/05/2025 23:18:18</t>
+    <t>09/05/2025 14:07:23</t>
+  </si>
+  <si>
+    <t>09/05/2025 12:39:56</t>
+  </si>
+  <si>
+    <t>08/05/2025 08:56:47</t>
+  </si>
+  <si>
+    <t>08/05/2025 08:10:05</t>
+  </si>
+  <si>
+    <t>Phúc Thọ</t>
   </si>
   <si>
     <t>Thạch Thất</t>
   </si>
   <si>
-    <t>Đan Phượng</t>
-  </si>
-  <si>
-    <t>Trạm smc mất điện - 1 - sonnn - 06/05/2025 23:24:34</t>
+    <t>Sơn Tây</t>
+  </si>
+  <si>
+    <t>184602- VTHN ĐKTĐ - Thay cột treo anten trạm , dự kiến từ 08h00 ngày 07/05 đến ngày 12/05 - 4 - hanhhh - 08/05/2025 09:17:21</t>
+  </si>
+  <si>
+    <t>184602- VTHN ĐKTĐ - Thay cột treo anten trạm , dự kiến từ 08h00 ngày 07/05 đến ngày 12/05  - 1 - hanhhh - 08/05/2025 08:54:42</t>
+  </si>
+  <si>
+    <t>Trạm viễn thông loại 2</t>
   </si>
   <si>
     <t>Trạm viễn thông loại 3</t>
+  </si>
+  <si>
+    <t>Trạm viễn thông loại 1</t>
   </si>
 </sst>
 </file>
@@ -503,7 +530,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC3"/>
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -515,7 +542,7 @@
     <col min="4" max="4" width="5.7109375" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
@@ -529,7 +556,7 @@
     <col min="19" max="19" width="9.7109375" customWidth="1"/>
     <col min="20" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="13.7109375" customWidth="1"/>
-    <col min="22" max="22" width="53.7109375" customWidth="1"/>
+    <col min="22" max="22" width="127.7109375" customWidth="1"/>
     <col min="23" max="23" width="12.7109375" customWidth="1"/>
     <col min="24" max="24" width="9.7109375" customWidth="1"/>
     <col min="25" max="25" width="12.7109375" customWidth="1"/>
@@ -638,16 +665,16 @@
         <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -657,7 +684,7 @@
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
@@ -666,7 +693,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AB2" s="2"/>
       <c r="AC2" s="2"/>
@@ -681,16 +708,16 @@
         <v>30</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -700,21 +727,109 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="U3" s="2"/>
-      <c r="V3" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AB3" s="2"/>
       <c r="AC3" s="2"/>
+    </row>
+    <row r="4" spans="1:29">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>